<commit_message>
Fixed File creation. Added labels to excel file. Corrected typos.
</commit_message>
<xml_diff>
--- a/excel_edge_list.xlsx
+++ b/excel_edge_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ASUFall2020\cse472\project1\code2\twitterNetworkVisualizer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C7BE6162-8BAE-4D92-BEF1-BF88C24408D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64D32AD4-B414-4C03-9AA7-689BBF2283A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0955ABB2-FB59-4118-9744-404EC55C4086}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="121">
   <si>
     <t>HIDEO_KOJIMA_EN</t>
   </si>
@@ -387,6 +387,15 @@
   </si>
   <si>
     <t>Jayne55927361</t>
+  </si>
+  <si>
+    <t>Node1</t>
+  </si>
+  <si>
+    <t>Node2</t>
+  </si>
+  <si>
+    <t>Edge List</t>
   </si>
 </sst>
 </file>
@@ -422,8 +431,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -738,10 +753,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46E95C3B-0F80-4A5B-9D9C-4FF3FDF011C9}">
-  <dimension ref="A1:B384"/>
+  <dimension ref="A1:B386"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -751,51 +766,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
+      <c r="A1" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
+      <c r="A2" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
         <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -803,7 +816,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -811,15 +824,15 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -827,15 +840,15 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
         <v>4</v>
-      </c>
-      <c r="B11" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -843,7 +856,7 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -851,15 +864,15 @@
         <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -867,15 +880,15 @@
         <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
         <v>4</v>
-      </c>
-      <c r="B16" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -883,7 +896,7 @@
         <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -891,23 +904,23 @@
         <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -915,15 +928,15 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
         <v>2</v>
-      </c>
-      <c r="B22" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -931,7 +944,7 @@
         <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -939,55 +952,55 @@
         <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B26" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
         <v>9</v>
-      </c>
-      <c r="B27" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B28" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B29" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -995,55 +1008,55 @@
         <v>12</v>
       </c>
       <c r="B31" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B32" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B33" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B35" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="B36" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37" t="s">
         <v>17</v>
-      </c>
-      <c r="B37" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
@@ -1051,31 +1064,31 @@
         <v>17</v>
       </c>
       <c r="B38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B39" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B40" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41" t="s">
         <v>20</v>
-      </c>
-      <c r="B41" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
@@ -1083,7 +1096,7 @@
         <v>20</v>
       </c>
       <c r="B42" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
@@ -1091,31 +1104,31 @@
         <v>20</v>
       </c>
       <c r="B43" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B44" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B45" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>8</v>
+      </c>
+      <c r="B46" t="s">
         <v>24</v>
-      </c>
-      <c r="B46" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
@@ -1123,7 +1136,7 @@
         <v>24</v>
       </c>
       <c r="B47" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
@@ -1131,31 +1144,31 @@
         <v>24</v>
       </c>
       <c r="B48" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
+        <v>24</v>
+      </c>
+      <c r="B49" t="s">
         <v>8</v>
-      </c>
-      <c r="B49" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B50" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
+        <v>8</v>
+      </c>
+      <c r="B51" t="s">
         <v>27</v>
-      </c>
-      <c r="B51" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
@@ -1163,7 +1176,7 @@
         <v>27</v>
       </c>
       <c r="B52" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
@@ -1171,55 +1184,55 @@
         <v>27</v>
       </c>
       <c r="B53" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="B54" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B55" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B56" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
+        <v>9</v>
+      </c>
+      <c r="B57" t="s">
         <v>10</v>
-      </c>
-      <c r="B57" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="B58" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
+        <v>10</v>
+      </c>
+      <c r="B59" t="s">
         <v>33</v>
-      </c>
-      <c r="B59" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
@@ -1227,7 +1240,7 @@
         <v>33</v>
       </c>
       <c r="B60" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
@@ -1235,31 +1248,31 @@
         <v>33</v>
       </c>
       <c r="B61" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="B62" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="B63" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
+        <v>10</v>
+      </c>
+      <c r="B64" t="s">
         <v>9</v>
-      </c>
-      <c r="B64" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
@@ -1267,23 +1280,23 @@
         <v>9</v>
       </c>
       <c r="B65" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
+        <v>9</v>
+      </c>
+      <c r="B66" t="s">
         <v>11</v>
-      </c>
-      <c r="B66" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="B67" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
@@ -1291,23 +1304,23 @@
         <v>11</v>
       </c>
       <c r="B68" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B69" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
+        <v>11</v>
+      </c>
+      <c r="B70" t="s">
         <v>39</v>
-      </c>
-      <c r="B70" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
@@ -1315,31 +1328,31 @@
         <v>39</v>
       </c>
       <c r="B71" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="B72" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B73" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
+        <v>11</v>
+      </c>
+      <c r="B74" t="s">
         <v>43</v>
-      </c>
-      <c r="B74" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
@@ -1347,7 +1360,7 @@
         <v>43</v>
       </c>
       <c r="B75" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
@@ -1355,47 +1368,47 @@
         <v>43</v>
       </c>
       <c r="B76" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="B77" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="B78" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B79" t="s">
-        <v>48</v>
+        <v>12</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="B80" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
+        <v>13</v>
+      </c>
+      <c r="B81" t="s">
         <v>48</v>
-      </c>
-      <c r="B81" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
@@ -1403,7 +1416,7 @@
         <v>48</v>
       </c>
       <c r="B82" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
@@ -1411,31 +1424,31 @@
         <v>48</v>
       </c>
       <c r="B83" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="B84" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="B85" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B86" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
@@ -1443,15 +1456,15 @@
         <v>12</v>
       </c>
       <c r="B87" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B88" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
@@ -1459,15 +1472,15 @@
         <v>12</v>
       </c>
       <c r="B89" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B90" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
@@ -1475,31 +1488,31 @@
         <v>12</v>
       </c>
       <c r="B91" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B92" t="s">
-        <v>53</v>
+        <v>14</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>53</v>
+        <v>12</v>
       </c>
       <c r="B93" t="s">
-        <v>54</v>
+        <v>15</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
+        <v>13</v>
+      </c>
+      <c r="B94" t="s">
         <v>53</v>
-      </c>
-      <c r="B94" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
@@ -1507,7 +1520,7 @@
         <v>53</v>
       </c>
       <c r="B95" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
@@ -1515,28 +1528,28 @@
         <v>53</v>
       </c>
       <c r="B96" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="B97" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="B98" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>58</v>
+        <v>12</v>
       </c>
       <c r="B99" t="s">
         <v>14</v>
@@ -1544,10 +1557,10 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
+        <v>14</v>
+      </c>
+      <c r="B100" t="s">
         <v>58</v>
-      </c>
-      <c r="B100" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
@@ -1563,31 +1576,31 @@
         <v>58</v>
       </c>
       <c r="B102" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
+        <v>58</v>
+      </c>
+      <c r="B103" t="s">
         <v>14</v>
-      </c>
-      <c r="B103" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B104" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
+        <v>14</v>
+      </c>
+      <c r="B105" t="s">
         <v>61</v>
-      </c>
-      <c r="B105" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
@@ -1595,7 +1608,7 @@
         <v>61</v>
       </c>
       <c r="B106" t="s">
-        <v>14</v>
+        <v>62</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
@@ -1603,31 +1616,31 @@
         <v>61</v>
       </c>
       <c r="B107" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
+        <v>61</v>
+      </c>
+      <c r="B108" t="s">
         <v>14</v>
-      </c>
-      <c r="B108" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B109" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
+        <v>14</v>
+      </c>
+      <c r="B110" t="s">
         <v>65</v>
-      </c>
-      <c r="B110" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
@@ -1635,7 +1648,7 @@
         <v>65</v>
       </c>
       <c r="B111" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
@@ -1643,23 +1656,23 @@
         <v>65</v>
       </c>
       <c r="B112" t="s">
-        <v>14</v>
+        <v>67</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="B113" t="s">
-        <v>15</v>
+        <v>68</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="B114" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
@@ -1667,15 +1680,15 @@
         <v>12</v>
       </c>
       <c r="B115" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B116" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
@@ -1683,87 +1696,87 @@
         <v>12</v>
       </c>
       <c r="B117" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B118" t="s">
-        <v>69</v>
+        <v>14</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
+        <v>12</v>
+      </c>
+      <c r="B119" t="s">
         <v>15</v>
-      </c>
-      <c r="B119" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="B120" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B121" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>71</v>
+        <v>1</v>
       </c>
       <c r="B122" t="s">
-        <v>72</v>
+        <v>16</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
+        <v>0</v>
+      </c>
+      <c r="B123" t="s">
         <v>71</v>
-      </c>
-      <c r="B123" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>12</v>
+        <v>71</v>
       </c>
       <c r="B124" t="s">
-        <v>13</v>
+        <v>72</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>13</v>
+        <v>71</v>
       </c>
       <c r="B125" t="s">
-        <v>48</v>
+        <v>12</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="B126" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
+        <v>13</v>
+      </c>
+      <c r="B127" t="s">
         <v>48</v>
-      </c>
-      <c r="B127" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
@@ -1771,7 +1784,7 @@
         <v>48</v>
       </c>
       <c r="B128" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
@@ -1779,31 +1792,31 @@
         <v>48</v>
       </c>
       <c r="B129" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="B130" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="B131" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B132" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.3">
@@ -1811,15 +1824,15 @@
         <v>12</v>
       </c>
       <c r="B133" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B134" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.3">
@@ -1827,15 +1840,15 @@
         <v>12</v>
       </c>
       <c r="B135" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B136" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
@@ -1843,31 +1856,31 @@
         <v>12</v>
       </c>
       <c r="B137" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B138" t="s">
-        <v>53</v>
+        <v>14</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>53</v>
+        <v>12</v>
       </c>
       <c r="B139" t="s">
-        <v>54</v>
+        <v>15</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
+        <v>13</v>
+      </c>
+      <c r="B140" t="s">
         <v>53</v>
-      </c>
-      <c r="B140" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.3">
@@ -1875,7 +1888,7 @@
         <v>53</v>
       </c>
       <c r="B141" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.3">
@@ -1883,28 +1896,28 @@
         <v>53</v>
       </c>
       <c r="B142" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="B143" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="B144" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>58</v>
+        <v>12</v>
       </c>
       <c r="B145" t="s">
         <v>14</v>
@@ -1912,10 +1925,10 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
+        <v>14</v>
+      </c>
+      <c r="B146" t="s">
         <v>58</v>
-      </c>
-      <c r="B146" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.3">
@@ -1931,31 +1944,31 @@
         <v>58</v>
       </c>
       <c r="B148" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
+        <v>58</v>
+      </c>
+      <c r="B149" t="s">
         <v>14</v>
-      </c>
-      <c r="B149" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B150" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
+        <v>14</v>
+      </c>
+      <c r="B151" t="s">
         <v>61</v>
-      </c>
-      <c r="B151" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.3">
@@ -1963,7 +1976,7 @@
         <v>61</v>
       </c>
       <c r="B152" t="s">
-        <v>14</v>
+        <v>62</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.3">
@@ -1971,31 +1984,31 @@
         <v>61</v>
       </c>
       <c r="B153" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
+        <v>61</v>
+      </c>
+      <c r="B154" t="s">
         <v>14</v>
-      </c>
-      <c r="B154" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B155" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
+        <v>14</v>
+      </c>
+      <c r="B156" t="s">
         <v>65</v>
-      </c>
-      <c r="B156" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.3">
@@ -2003,7 +2016,7 @@
         <v>65</v>
       </c>
       <c r="B157" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.3">
@@ -2011,23 +2024,23 @@
         <v>65</v>
       </c>
       <c r="B158" t="s">
-        <v>14</v>
+        <v>67</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="B159" t="s">
-        <v>15</v>
+        <v>68</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="B160" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.3">
@@ -2035,15 +2048,15 @@
         <v>12</v>
       </c>
       <c r="B161" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B162" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.3">
@@ -2051,60 +2064,60 @@
         <v>12</v>
       </c>
       <c r="B163" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B164" t="s">
-        <v>69</v>
+        <v>14</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
+        <v>12</v>
+      </c>
+      <c r="B165" t="s">
         <v>15</v>
-      </c>
-      <c r="B165" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>71</v>
+        <v>15</v>
       </c>
       <c r="B166" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>71</v>
+        <v>15</v>
       </c>
       <c r="B167" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B168" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>36</v>
+        <v>71</v>
       </c>
       <c r="B169" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B170" t="s">
         <v>36</v>
@@ -2112,10 +2125,10 @@
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
+        <v>36</v>
+      </c>
+      <c r="B171" t="s">
         <v>75</v>
-      </c>
-      <c r="B171" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.3">
@@ -2131,31 +2144,31 @@
         <v>75</v>
       </c>
       <c r="B173" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
+        <v>75</v>
+      </c>
+      <c r="B174" t="s">
         <v>36</v>
-      </c>
-      <c r="B174" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B175" t="s">
-        <v>78</v>
+        <v>36</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
+        <v>36</v>
+      </c>
+      <c r="B176" t="s">
         <v>77</v>
-      </c>
-      <c r="B176" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.3">
@@ -2163,7 +2176,7 @@
         <v>77</v>
       </c>
       <c r="B177" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.3">
@@ -2176,26 +2189,26 @@
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>36</v>
+        <v>77</v>
       </c>
       <c r="B179" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B180" t="s">
-        <v>81</v>
+        <v>36</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
+        <v>36</v>
+      </c>
+      <c r="B181" t="s">
         <v>80</v>
-      </c>
-      <c r="B181" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.3">
@@ -2203,7 +2216,7 @@
         <v>80</v>
       </c>
       <c r="B182" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.3">
@@ -2211,44 +2224,44 @@
         <v>80</v>
       </c>
       <c r="B183" t="s">
-        <v>36</v>
+        <v>82</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>36</v>
+        <v>80</v>
       </c>
       <c r="B184" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B185" t="s">
-        <v>85</v>
+        <v>36</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>74</v>
+        <v>36</v>
       </c>
       <c r="B186" t="s">
-        <v>36</v>
+        <v>84</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>36</v>
+        <v>84</v>
       </c>
       <c r="B187" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B188" t="s">
         <v>36</v>
@@ -2256,10 +2269,10 @@
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
+        <v>36</v>
+      </c>
+      <c r="B189" t="s">
         <v>75</v>
-      </c>
-      <c r="B189" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.3">
@@ -2275,31 +2288,31 @@
         <v>75</v>
       </c>
       <c r="B191" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
+        <v>75</v>
+      </c>
+      <c r="B192" t="s">
         <v>36</v>
-      </c>
-      <c r="B192" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B193" t="s">
-        <v>78</v>
+        <v>36</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
+        <v>36</v>
+      </c>
+      <c r="B194" t="s">
         <v>77</v>
-      </c>
-      <c r="B194" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.3">
@@ -2307,7 +2320,7 @@
         <v>77</v>
       </c>
       <c r="B195" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.3">
@@ -2320,26 +2333,26 @@
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>36</v>
+        <v>77</v>
       </c>
       <c r="B197" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B198" t="s">
-        <v>81</v>
+        <v>36</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
+        <v>36</v>
+      </c>
+      <c r="B199" t="s">
         <v>80</v>
-      </c>
-      <c r="B199" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.3">
@@ -2347,7 +2360,7 @@
         <v>80</v>
       </c>
       <c r="B200" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.3">
@@ -2355,55 +2368,55 @@
         <v>80</v>
       </c>
       <c r="B201" t="s">
-        <v>36</v>
+        <v>82</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>36</v>
+        <v>80</v>
       </c>
       <c r="B202" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B203" t="s">
-        <v>85</v>
+        <v>36</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>74</v>
+        <v>36</v>
       </c>
       <c r="B204" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B205" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="B206" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
+        <v>86</v>
+      </c>
+      <c r="B207" t="s">
         <v>87</v>
-      </c>
-      <c r="B207" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.3">
@@ -2411,31 +2424,31 @@
         <v>87</v>
       </c>
       <c r="B208" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B209" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B210" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
+        <v>86</v>
+      </c>
+      <c r="B211" t="s">
         <v>91</v>
-      </c>
-      <c r="B211" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.3">
@@ -2443,7 +2456,7 @@
         <v>91</v>
       </c>
       <c r="B212" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.3">
@@ -2451,31 +2464,31 @@
         <v>91</v>
       </c>
       <c r="B213" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B214" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B215" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
+        <v>86</v>
+      </c>
+      <c r="B216" t="s">
         <v>95</v>
-      </c>
-      <c r="B216" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.3">
@@ -2483,55 +2496,55 @@
         <v>95</v>
       </c>
       <c r="B217" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="B218" t="s">
-        <v>1</v>
+        <v>97</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>1</v>
+        <v>95</v>
       </c>
       <c r="B219" t="s">
-        <v>2</v>
+        <v>98</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B220" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B221" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B222" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
+        <v>3</v>
+      </c>
+      <c r="B223" t="s">
         <v>4</v>
-      </c>
-      <c r="B223" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.3">
@@ -2539,7 +2552,7 @@
         <v>4</v>
       </c>
       <c r="B224" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.3">
@@ -2547,15 +2560,15 @@
         <v>4</v>
       </c>
       <c r="B225" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B226" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.3">
@@ -2563,15 +2576,15 @@
         <v>4</v>
       </c>
       <c r="B227" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
+        <v>3</v>
+      </c>
+      <c r="B228" t="s">
         <v>4</v>
-      </c>
-      <c r="B228" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.3">
@@ -2579,7 +2592,7 @@
         <v>4</v>
       </c>
       <c r="B229" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.3">
@@ -2587,15 +2600,15 @@
         <v>4</v>
       </c>
       <c r="B230" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B231" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.3">
@@ -2603,15 +2616,15 @@
         <v>4</v>
       </c>
       <c r="B232" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
+        <v>3</v>
+      </c>
+      <c r="B233" t="s">
         <v>4</v>
-      </c>
-      <c r="B233" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.3">
@@ -2619,7 +2632,7 @@
         <v>4</v>
       </c>
       <c r="B234" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.3">
@@ -2627,23 +2640,23 @@
         <v>4</v>
       </c>
       <c r="B235" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B236" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B237" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.3">
@@ -2651,15 +2664,15 @@
         <v>2</v>
       </c>
       <c r="B238" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
+        <v>1</v>
+      </c>
+      <c r="B239" t="s">
         <v>2</v>
-      </c>
-      <c r="B239" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.3">
@@ -2667,7 +2680,7 @@
         <v>2</v>
       </c>
       <c r="B240" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.3">
@@ -2675,55 +2688,55 @@
         <v>2</v>
       </c>
       <c r="B241" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B242" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B243" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
+        <v>1</v>
+      </c>
+      <c r="B244" t="s">
         <v>9</v>
-      </c>
-      <c r="B244" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B245" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B246" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B247" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.3">
@@ -2731,55 +2744,55 @@
         <v>12</v>
       </c>
       <c r="B248" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B249" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B250" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B251" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B252" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="B253" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
+        <v>8</v>
+      </c>
+      <c r="B254" t="s">
         <v>17</v>
-      </c>
-      <c r="B254" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.3">
@@ -2787,31 +2800,31 @@
         <v>17</v>
       </c>
       <c r="B255" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B256" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B257" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
+        <v>8</v>
+      </c>
+      <c r="B258" t="s">
         <v>20</v>
-      </c>
-      <c r="B258" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.3">
@@ -2819,7 +2832,7 @@
         <v>20</v>
       </c>
       <c r="B259" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.3">
@@ -2827,31 +2840,31 @@
         <v>20</v>
       </c>
       <c r="B260" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B261" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B262" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
+        <v>8</v>
+      </c>
+      <c r="B263" t="s">
         <v>24</v>
-      </c>
-      <c r="B263" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.3">
@@ -2859,7 +2872,7 @@
         <v>24</v>
       </c>
       <c r="B264" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.3">
@@ -2867,31 +2880,31 @@
         <v>24</v>
       </c>
       <c r="B265" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
+        <v>24</v>
+      </c>
+      <c r="B266" t="s">
         <v>8</v>
-      </c>
-      <c r="B266" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B267" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
+        <v>8</v>
+      </c>
+      <c r="B268" t="s">
         <v>27</v>
-      </c>
-      <c r="B268" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.3">
@@ -2899,7 +2912,7 @@
         <v>27</v>
       </c>
       <c r="B269" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.3">
@@ -2907,55 +2920,55 @@
         <v>27</v>
       </c>
       <c r="B270" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="B271" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B272" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B273" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
+        <v>9</v>
+      </c>
+      <c r="B274" t="s">
         <v>10</v>
-      </c>
-      <c r="B274" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="B275" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
+        <v>10</v>
+      </c>
+      <c r="B276" t="s">
         <v>33</v>
-      </c>
-      <c r="B276" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.3">
@@ -2963,7 +2976,7 @@
         <v>33</v>
       </c>
       <c r="B277" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.3">
@@ -2971,31 +2984,31 @@
         <v>33</v>
       </c>
       <c r="B278" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="B279" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="B280" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
+        <v>10</v>
+      </c>
+      <c r="B281" t="s">
         <v>9</v>
-      </c>
-      <c r="B281" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.3">
@@ -3003,23 +3016,23 @@
         <v>9</v>
       </c>
       <c r="B282" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
+        <v>9</v>
+      </c>
+      <c r="B283" t="s">
         <v>11</v>
-      </c>
-      <c r="B283" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="B284" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.3">
@@ -3027,23 +3040,23 @@
         <v>11</v>
       </c>
       <c r="B285" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B286" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
+        <v>11</v>
+      </c>
+      <c r="B287" t="s">
         <v>39</v>
-      </c>
-      <c r="B287" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.3">
@@ -3051,31 +3064,31 @@
         <v>39</v>
       </c>
       <c r="B288" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="B289" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B290" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
+        <v>11</v>
+      </c>
+      <c r="B291" t="s">
         <v>43</v>
-      </c>
-      <c r="B291" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.3">
@@ -3083,7 +3096,7 @@
         <v>43</v>
       </c>
       <c r="B292" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.3">
@@ -3091,47 +3104,47 @@
         <v>43</v>
       </c>
       <c r="B293" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="B294" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="B295" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B296" t="s">
-        <v>48</v>
+        <v>12</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="B297" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
+        <v>13</v>
+      </c>
+      <c r="B298" t="s">
         <v>48</v>
-      </c>
-      <c r="B298" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.3">
@@ -3139,7 +3152,7 @@
         <v>48</v>
       </c>
       <c r="B299" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.3">
@@ -3147,31 +3160,31 @@
         <v>48</v>
       </c>
       <c r="B300" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="B301" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="B302" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B303" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.3">
@@ -3179,15 +3192,15 @@
         <v>12</v>
       </c>
       <c r="B304" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B305" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.3">
@@ -3195,15 +3208,15 @@
         <v>12</v>
       </c>
       <c r="B306" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B307" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.3">
@@ -3211,31 +3224,31 @@
         <v>12</v>
       </c>
       <c r="B308" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B309" t="s">
-        <v>53</v>
+        <v>14</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
-        <v>53</v>
+        <v>12</v>
       </c>
       <c r="B310" t="s">
-        <v>54</v>
+        <v>15</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
+        <v>13</v>
+      </c>
+      <c r="B311" t="s">
         <v>53</v>
-      </c>
-      <c r="B311" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.3">
@@ -3243,7 +3256,7 @@
         <v>53</v>
       </c>
       <c r="B312" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.3">
@@ -3251,28 +3264,28 @@
         <v>53</v>
       </c>
       <c r="B313" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="B314" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="B315" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
-        <v>58</v>
+        <v>12</v>
       </c>
       <c r="B316" t="s">
         <v>14</v>
@@ -3280,10 +3293,10 @@
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
+        <v>14</v>
+      </c>
+      <c r="B317" t="s">
         <v>58</v>
-      </c>
-      <c r="B317" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.3">
@@ -3299,31 +3312,31 @@
         <v>58</v>
       </c>
       <c r="B319" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
+        <v>58</v>
+      </c>
+      <c r="B320" t="s">
         <v>14</v>
-      </c>
-      <c r="B320" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B321" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
+        <v>14</v>
+      </c>
+      <c r="B322" t="s">
         <v>61</v>
-      </c>
-      <c r="B322" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.3">
@@ -3331,7 +3344,7 @@
         <v>61</v>
       </c>
       <c r="B323" t="s">
-        <v>14</v>
+        <v>62</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.3">
@@ -3339,31 +3352,31 @@
         <v>61</v>
       </c>
       <c r="B324" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
+        <v>61</v>
+      </c>
+      <c r="B325" t="s">
         <v>14</v>
-      </c>
-      <c r="B325" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B326" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
+        <v>14</v>
+      </c>
+      <c r="B327" t="s">
         <v>65</v>
-      </c>
-      <c r="B327" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.3">
@@ -3371,7 +3384,7 @@
         <v>65</v>
       </c>
       <c r="B328" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.3">
@@ -3379,23 +3392,23 @@
         <v>65</v>
       </c>
       <c r="B329" t="s">
-        <v>14</v>
+        <v>67</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="B330" t="s">
-        <v>15</v>
+        <v>68</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="B331" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.3">
@@ -3403,15 +3416,15 @@
         <v>12</v>
       </c>
       <c r="B332" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B333" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.3">
@@ -3419,79 +3432,79 @@
         <v>12</v>
       </c>
       <c r="B334" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B335" t="s">
-        <v>69</v>
+        <v>14</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
+        <v>12</v>
+      </c>
+      <c r="B336" t="s">
         <v>15</v>
-      </c>
-      <c r="B336" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="B337" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B338" t="s">
-        <v>99</v>
+        <v>70</v>
       </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
-        <v>99</v>
+        <v>1</v>
       </c>
       <c r="B339" t="s">
-        <v>100</v>
+        <v>16</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="B340" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B341" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B342" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
+        <v>101</v>
+      </c>
+      <c r="B343" t="s">
         <v>102</v>
-      </c>
-      <c r="B343" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.3">
@@ -3507,39 +3520,39 @@
         <v>102</v>
       </c>
       <c r="B345" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B346" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B347" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B348" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
+        <v>105</v>
+      </c>
+      <c r="B349" t="s">
         <v>106</v>
-      </c>
-      <c r="B349" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.3">
@@ -3547,7 +3560,7 @@
         <v>106</v>
       </c>
       <c r="B350" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.3">
@@ -3555,31 +3568,31 @@
         <v>106</v>
       </c>
       <c r="B351" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B352" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A353" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B353" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A354" t="s">
+        <v>105</v>
+      </c>
+      <c r="B354" t="s">
         <v>111</v>
-      </c>
-      <c r="B354" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.3">
@@ -3587,7 +3600,7 @@
         <v>111</v>
       </c>
       <c r="B355" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.3">
@@ -3600,7 +3613,7 @@
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A357" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B357" t="s">
         <v>113</v>
@@ -3608,18 +3621,18 @@
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A358" t="s">
+        <v>111</v>
+      </c>
+      <c r="B358" t="s">
         <v>113</v>
-      </c>
-      <c r="B358" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A359" t="s">
+        <v>105</v>
+      </c>
+      <c r="B359" t="s">
         <v>113</v>
-      </c>
-      <c r="B359" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.3">
@@ -3627,7 +3640,7 @@
         <v>113</v>
       </c>
       <c r="B360" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.3">
@@ -3635,15 +3648,15 @@
         <v>113</v>
       </c>
       <c r="B361" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A362" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="B362" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.3">
@@ -3651,15 +3664,15 @@
         <v>113</v>
       </c>
       <c r="B363" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A364" t="s">
+        <v>105</v>
+      </c>
+      <c r="B364" t="s">
         <v>113</v>
-      </c>
-      <c r="B364" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.3">
@@ -3667,7 +3680,7 @@
         <v>113</v>
       </c>
       <c r="B365" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.3">
@@ -3675,31 +3688,31 @@
         <v>113</v>
       </c>
       <c r="B366" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A367" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="B367" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A368" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B368" t="s">
-        <v>99</v>
+        <v>116</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A369" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B369" t="s">
-        <v>100</v>
+        <v>117</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.3">
@@ -3723,15 +3736,15 @@
         <v>117</v>
       </c>
       <c r="B372" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A373" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B373" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.3">
@@ -3739,39 +3752,39 @@
         <v>117</v>
       </c>
       <c r="B374" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A375" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B375" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A376" t="s">
-        <v>100</v>
+        <v>117</v>
       </c>
       <c r="B376" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A377" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="B377" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A378" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B378" t="s">
-        <v>100</v>
+        <v>117</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.3">
@@ -3795,15 +3808,15 @@
         <v>117</v>
       </c>
       <c r="B381" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A382" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B382" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.3">
@@ -3811,18 +3824,38 @@
         <v>117</v>
       </c>
       <c r="B383" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A384" t="s">
+        <v>101</v>
+      </c>
+      <c r="B384" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="385" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A385" t="s">
+        <v>117</v>
+      </c>
+      <c r="B385" t="s">
         <v>99</v>
       </c>
-      <c r="B384" t="s">
+    </row>
+    <row r="386" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A386" t="s">
+        <v>99</v>
+      </c>
+      <c r="B386" t="s">
         <v>100</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>